<commit_message>
update files via auto commit
</commit_message>
<xml_diff>
--- a/ТВИМС/2/LR2_Regressia (1).xlsx
+++ b/ТВИМС/2/LR2_Regressia (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Force\Documents\University\3sem\ТВИМС\2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54F03993-86F0-4A97-9AA9-7A68BEB11D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C815FE-8C0A-4936-B20C-0A722E13EE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,19 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>Выборочный коэффициент корреляции</t>
-  </si>
-  <si>
-    <t>t расч</t>
-  </si>
-  <si>
-    <t>критерия Стьюдента:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>xi</t>
   </si>
@@ -58,69 +46,6 @@
   </si>
   <si>
     <t>yi^2</t>
-  </si>
-  <si>
-    <t>t табл</t>
-  </si>
-  <si>
-    <t>квантилей распределения Стьюдента</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Поскольку </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>расч &gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> табл то при уровне значимости α = 0,05 коэффициент корреляции считаем значимо отличающимся от нуля, а следовательно, связь между величинами x, y признается статистически значимой.</t>
-    </r>
-  </si>
-  <si>
-    <t>Поскольку коэффициент корреляции признается значимо отличающимся от нуля, можно принять предположение о линейной регрессионной зависимости между наблюдаемыми величинами</t>
   </si>
   <si>
     <t>n=</t>
@@ -256,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,14 +215,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
@@ -530,9 +447,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -581,11 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -597,23 +510,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -6593,7 +6509,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>696076</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>173355</xdr:rowOff>
+      <xdr:rowOff>173356</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6817,15 +6733,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>136072</xdr:colOff>
+      <xdr:colOff>136071</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>73269</xdr:rowOff>
+      <xdr:rowOff>51865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>531726</xdr:colOff>
+      <xdr:colOff>531725</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>21771</xdr:rowOff>
+      <xdr:rowOff>64581</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7193,10 +7109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y63"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="89" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="89" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7213,16 +7129,16 @@
     <col min="16" max="16" width="12.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
-      <c r="A1" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+    <row r="1" spans="1:17">
+      <c r="A1" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75">
+    <row r="2" spans="1:17" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -7252,9 +7168,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.75">
+    <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2">
         <v>19</v>
@@ -7283,54 +7199,34 @@
       <c r="J3" s="2">
         <v>78</v>
       </c>
-      <c r="X3" t="s">
+    </row>
+    <row r="5" spans="1:17" ht="15.75">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:25">
-      <c r="X4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="15.75">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>43</v>
-      </c>
-      <c r="X5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="15.75">
+    <row r="6" spans="1:17" ht="15.75">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -7349,20 +7245,20 @@
         <f>POWER(B6,2)</f>
         <v>361</v>
       </c>
-      <c r="F6" s="49">
+      <c r="F6" s="47">
         <v>1</v>
       </c>
       <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" t="s">
         <v>37</v>
       </c>
-      <c r="N6" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75">
+    <row r="7" spans="1:17" ht="15.75">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -7385,16 +7281,16 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="N7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="Q7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="21">
+    <row r="8" spans="1:17" ht="15.75">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -7416,17 +7312,14 @@
       <c r="F8" s="45">
         <v>3</v>
       </c>
-      <c r="M8" s="50" t="s">
-        <v>41</v>
+      <c r="M8" s="48" t="s">
+        <v>33</v>
       </c>
       <c r="N8" t="s">
-        <v>42</v>
-      </c>
-      <c r="X8" s="46" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75">
+    <row r="9" spans="1:17" ht="15.75">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -7449,7 +7342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15.75">
+    <row r="10" spans="1:17" ht="15.75">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -7471,11 +7364,8 @@
       <c r="F10" s="45">
         <v>5</v>
       </c>
-      <c r="X10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="11" spans="1:25" ht="15.75">
+    <row r="11" spans="1:17" ht="15.75">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -7498,7 +7388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75">
+    <row r="12" spans="1:17" ht="15.75">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -7521,7 +7411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15.75">
+    <row r="13" spans="1:17" ht="15.75">
       <c r="A13" s="2">
         <v>7</v>
       </c>
@@ -7544,7 +7434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15.75">
+    <row r="14" spans="1:17" ht="15.75">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -7567,10 +7457,10 @@
         <v>9</v>
       </c>
       <c r="M14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="29.25" customHeight="1">
+    <row r="15" spans="1:17" ht="29.25" customHeight="1">
       <c r="A15" s="5">
         <f>SUM(A6:A14)</f>
         <v>36</v>
@@ -7591,13 +7481,13 @@
         <f>SUM(E6:E14)</f>
         <v>18973</v>
       </c>
-      <c r="F15" s="48" t="s">
-        <v>47</v>
+      <c r="F15" s="46" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:17">
       <c r="A16" s="6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B16" s="6">
         <f>COUNT(A6:A14)</f>
@@ -7606,21 +7496,21 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B17" s="8">
         <f>CORREL(A6:A14,B6:B14)</f>
         <v>0.96623451166765173</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D17" s="10">
         <f>ABS(B17)*SQRT((B16-2)/(1-B17^2))</f>
         <v>9.9215012303703798</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F17" s="12">
         <v>2.36</v>
@@ -7628,13 +7518,13 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="50" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="L19" s="48" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -7650,11 +7540,11 @@
         <f>B15</f>
         <v>371</v>
       </c>
-      <c r="L20" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="M20" s="52" t="s">
-        <v>49</v>
+      <c r="L20" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="M20" s="50" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -7670,21 +7560,21 @@
         <f>C15</f>
         <v>1938</v>
       </c>
-      <c r="L21" s="53">
+      <c r="L21" s="51">
         <f>A6</f>
         <v>0</v>
       </c>
-      <c r="M21" s="53">
+      <c r="M21" s="51">
         <f>1/B6</f>
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="L22" s="53">
-        <f t="shared" ref="L22:L30" si="3">A7</f>
+      <c r="L22" s="51">
+        <f t="shared" ref="L22:L29" si="3">A7</f>
         <v>1</v>
       </c>
-      <c r="M22" s="53">
+      <c r="M22" s="51">
         <f t="shared" ref="M22:M29" si="4">1/B7</f>
         <v>4.7619047619047616E-2</v>
       </c>
@@ -7698,17 +7588,17 @@
         <v>-6.6666666666666666E-2</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D23" s="20">
         <f t="array" ref="D23:D24">MMULT(A23:B24,D20:D21)</f>
         <v>10.955555555555577</v>
       </c>
-      <c r="L23" s="53">
+      <c r="L23" s="51">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M23" s="53">
+      <c r="M23" s="51">
         <f t="shared" si="4"/>
         <v>4.3478260869565216E-2</v>
       </c>
@@ -7721,55 +7611,55 @@
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D24" s="22">
         <v>7.5666666666666629</v>
       </c>
-      <c r="L24" s="53">
+      <c r="L24" s="51">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="M24" s="53">
+      <c r="M24" s="51">
         <f t="shared" si="4"/>
         <v>3.5714285714285712E-2</v>
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="L25" s="53">
+      <c r="L25" s="51">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="M25" s="53">
+      <c r="M25" s="51">
         <f t="shared" si="4"/>
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="L26" s="53">
+        <v>13</v>
+      </c>
+      <c r="L26" s="51">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="M26" s="53">
+      <c r="M26" s="51">
         <f t="shared" si="4"/>
         <v>2.1739130434782608E-2</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75">
       <c r="A27" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L27" s="53">
+        <v>1</v>
+      </c>
+      <c r="L27" s="51">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M27" s="53">
+      <c r="M27" s="51">
         <f t="shared" si="4"/>
         <v>1.6666666666666666E-2</v>
       </c>
@@ -7782,11 +7672,11 @@
         <f>$D$23+$D$24*A28</f>
         <v>10.955555555555577</v>
       </c>
-      <c r="L28" s="53">
+      <c r="L28" s="51">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="M28" s="53">
+      <c r="M28" s="51">
         <f t="shared" si="4"/>
         <v>1.5873015873015872E-2</v>
       </c>
@@ -7799,11 +7689,11 @@
         <f t="shared" ref="B29:B36" si="5">$D$23+$D$24*A29</f>
         <v>18.52222222222224</v>
       </c>
-      <c r="L29" s="53">
+      <c r="L29" s="51">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="M29" s="53">
+      <c r="M29" s="51">
         <f t="shared" si="4"/>
         <v>1.282051282051282E-2</v>
       </c>
@@ -7871,15 +7761,15 @@
         <v>71.48888888888888</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="50" t="s">
-        <v>48</v>
+        <v>14</v>
+      </c>
+      <c r="D36" s="48" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E39" s="23"/>
       <c r="F39" s="23"/>
@@ -7887,25 +7777,25 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="25" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -7937,7 +7827,7 @@
         <f>B41*E41</f>
         <v>0</v>
       </c>
-      <c r="H41" s="49">
+      <c r="H41" s="47">
         <v>1</v>
       </c>
     </row>
@@ -7967,7 +7857,7 @@
         <v>21</v>
       </c>
       <c r="G42" s="27">
-        <f t="shared" ref="G41:G50" si="12">B42*E42</f>
+        <f t="shared" ref="G42:G50" si="12">B42*E42</f>
         <v>21</v>
       </c>
       <c r="H42" s="45">
@@ -8207,7 +8097,7 @@
     </row>
     <row r="50" spans="1:13" ht="27" customHeight="1">
       <c r="A50" s="28">
-        <f t="shared" ref="A50:G50" si="13">SUM(A41:A49)</f>
+        <f t="shared" ref="A50:F50" si="13">SUM(A41:A49)</f>
         <v>36</v>
       </c>
       <c r="B50" s="29">
@@ -8234,13 +8124,13 @@
         <f t="shared" si="12"/>
         <v>75684</v>
       </c>
-      <c r="H50" s="68" t="s">
-        <v>47</v>
+      <c r="H50" s="66" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B51" s="6">
         <f>COUNT(A41:A49)</f>
@@ -8249,21 +8139,21 @@
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B52" s="8">
         <f>CORREL(A41:A49,E41:E49)</f>
         <v>0.96623451166765173</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D52" s="10">
         <f>ABS(B52)*SQRT((B51-2)/(1-B52^2))</f>
         <v>9.9215012303703798</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F52" s="12">
         <v>2.36</v>
@@ -8271,27 +8161,27 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" thickBot="1">
       <c r="A54" t="s">
-        <v>17</v>
-      </c>
-      <c r="L54" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="L54" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="M54" s="47" t="s">
         <v>46</v>
-      </c>
-      <c r="M54" s="49" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="57">
+      <c r="A55" s="55">
         <v>9</v>
       </c>
-      <c r="B55" s="61">
+      <c r="B55" s="59">
         <v>36</v>
       </c>
-      <c r="C55" s="58">
+      <c r="C55" s="56">
         <v>204</v>
       </c>
-      <c r="D55" s="54"/>
-      <c r="E55" s="55">
+      <c r="D55" s="52"/>
+      <c r="E55" s="53">
         <v>371</v>
       </c>
       <c r="L55" s="27">
@@ -8304,17 +8194,17 @@
       </c>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="62">
+      <c r="A56" s="60">
         <v>36</v>
       </c>
-      <c r="B56" s="63">
+      <c r="B56" s="61">
         <v>204</v>
       </c>
-      <c r="C56" s="64">
+      <c r="C56" s="62">
         <v>1296</v>
       </c>
-      <c r="D56" s="54"/>
-      <c r="E56" s="66">
+      <c r="D56" s="52"/>
+      <c r="E56" s="64">
         <v>1938</v>
       </c>
       <c r="L56" s="27">
@@ -8327,17 +8217,17 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A57" s="59">
+      <c r="A57" s="57">
         <v>204</v>
       </c>
-      <c r="B57" s="65">
+      <c r="B57" s="63">
         <v>1296</v>
       </c>
-      <c r="C57" s="60">
+      <c r="C57" s="58">
         <v>8772</v>
       </c>
-      <c r="D57" s="54"/>
-      <c r="E57" s="56">
+      <c r="D57" s="52"/>
+      <c r="E57" s="54">
         <v>75684</v>
       </c>
       <c r="L57" s="27">
@@ -8371,8 +8261,8 @@
       <c r="C59" s="35">
         <v>3.0303030303030311E-2</v>
       </c>
-      <c r="D59" s="67" t="s">
-        <v>51</v>
+      <c r="D59" s="65" t="s">
+        <v>43</v>
       </c>
       <c r="E59" s="36">
         <f t="array" ref="E59:E61">MMULT(A59:C61,E55:E57)</f>
@@ -8398,8 +8288,8 @@
       <c r="C60" s="38">
         <v>-2.5974025974026003E-2</v>
       </c>
-      <c r="D60" s="51" t="s">
-        <v>52</v>
+      <c r="D60" s="49" t="s">
+        <v>44</v>
       </c>
       <c r="E60" s="40">
         <v>-1645.4896103896122</v>
@@ -8423,8 +8313,8 @@
       <c r="C61" s="43">
         <v>3.2467532467532509E-3</v>
       </c>
-      <c r="D61" s="51" t="s">
-        <v>53</v>
+      <c r="D61" s="49" t="s">
+        <v>45</v>
       </c>
       <c r="E61" s="44">
         <v>206.6320346320349</v>
@@ -8462,7 +8352,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>